<commit_message>
fix revise bug, add color on download excel, fix filter bug
</commit_message>
<xml_diff>
--- a/dashboard/static/reportSave/table_result.xlsx
+++ b/dashboard/static/reportSave/table_result.xlsx
@@ -1,37 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>题目数量</t>
+  </si>
+  <si>
+    <t>1（%）</t>
+  </si>
+  <si>
+    <t>2（%）</t>
+  </si>
+  <si>
+    <t>3（%）</t>
+  </si>
+  <si>
+    <t>4（%）</t>
+  </si>
+  <si>
+    <t>合格率</t>
+  </si>
+  <si>
+    <t>整体结果</t>
+  </si>
+  <si>
+    <t>民族歧视</t>
+  </si>
+  <si>
+    <t>信仰歧视</t>
+  </si>
+  <si>
+    <t>国别歧视</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +84,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,152 +400,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>题目数量</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>1（%）</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2（%）</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>3（%）</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>4（%）</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>合格率</t>
-        </is>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>整体结果</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="C2">
         <v>40</v>
       </c>
-      <c r="G2" t="n">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>60</v>
       </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>民族歧视</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>50</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>50</v>
       </c>
-      <c r="G3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>信仰歧视</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>100</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>国别歧视</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>50</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>50</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix audit revise page error
</commit_message>
<xml_diff>
--- a/dashboard/static/reportSave/table_result.xlsx
+++ b/dashboard/static/reportSave/table_result.xlsx
@@ -19,18 +19,6 @@
     <t>题目数量</t>
   </si>
   <si>
-    <t>1（%）</t>
-  </si>
-  <si>
-    <t>2（%）</t>
-  </si>
-  <si>
-    <t>3（%）</t>
-  </si>
-  <si>
-    <t>4（%）</t>
-  </si>
-  <si>
     <t>合格率</t>
   </si>
   <si>
@@ -44,6 +32,18 @@
   </si>
   <si>
     <t>国别歧视</t>
+  </si>
+  <si>
+    <t>60.0%</t>
+  </si>
+  <si>
+    <t>100.0%</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
+    <t>50.0%</t>
   </si>
 </sst>
 </file>
@@ -411,31 +411,31 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -444,15 +444,15 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>60</v>
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -467,21 +467,21 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -492,19 +492,19 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -513,10 +513,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>50</v>
-      </c>
-      <c r="G5">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>